<commit_message>
Created Feature space and working on it
</commit_message>
<xml_diff>
--- a/Task1/Test.xlsx
+++ b/Task1/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12AC4E0-E034-46A4-B442-28195E891E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5EBA50D-9ADA-4CF3-9DAD-199D47252E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="33">
   <si>
     <t>Path</t>
   </si>
@@ -37,12 +37,6 @@
     <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Unknown- Test split\Cropped\adolf-hitler-photo-u53.jpg</t>
   </si>
   <si>
-    <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Unknown- Test split\Cropped\download.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Unknown- Test split\Cropped\idi-amin-u4.jpg</t>
-  </si>
-  <si>
     <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Unknown- Test split\Cropped\images.jpg</t>
   </si>
   <si>
@@ -85,16 +79,10 @@
     <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Sameed - Test split\Cropped\IMG_20230305_175454.jpg</t>
   </si>
   <si>
-    <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Sameed - Test split\Cropped\IMG_20230305_175457.jpg</t>
-  </si>
-  <si>
     <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Sameed - Test split\Cropped\IMG_20230305_175503.jpg</t>
   </si>
   <si>
     <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Sameed - Test split\Cropped\IMG_20230305_175505.jpg</t>
-  </si>
-  <si>
-    <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Sameed - Test split\Cropped\IMG_20230305_175508.jpg</t>
   </si>
   <si>
     <t>C:\Users\Sameed\Desktop\Machine-Learning-Ass-1\Task1\Sameed - Test split\Cropped\IMG_20230305_175515.jpg</t>
@@ -971,10 +959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,10 +991,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>56</v>
@@ -1017,13 +1005,13 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1031,13 +1019,13 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
       <c r="D4">
-        <v>78</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1045,13 +1033,13 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>82</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,13 +1047,13 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D6">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1073,13 +1061,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1087,10 +1075,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8">
         <v>69</v>
@@ -1101,52 +1089,66 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D9">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D10">
-        <v>69</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D11">
-        <v>70</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>22</v>
@@ -1154,13 +1156,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14">
         <v>22</v>
@@ -1168,13 +1170,13 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <v>22</v>
@@ -1182,13 +1184,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>22</v>
@@ -1196,13 +1198,13 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>22</v>
@@ -1210,13 +1212,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>22</v>
@@ -1224,13 +1226,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>22</v>
@@ -1238,13 +1240,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D20">
         <v>22</v>
@@ -1252,13 +1254,13 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>22</v>
@@ -1266,27 +1268,41 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D22">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D24">
         <v>22</v>
@@ -1294,99 +1310,15 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D25">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>30</v>
-      </c>
-      <c r="B26" t="s">
-        <v>36</v>
-      </c>
-      <c r="C26" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" t="s">
-        <v>15</v>
-      </c>
-      <c r="D27">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>32</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>33</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D29">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>15</v>
-      </c>
-      <c r="D30">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31">
         <v>22</v>
       </c>
     </row>

</xml_diff>